<commit_message>
Stuck in a Rut
</commit_message>
<xml_diff>
--- a/myCpps_2020/USACO2020DecSilverRectangularPasture/USACO2020DecSilverRectangularPasture.xlsx
+++ b/myCpps_2020/USACO2020DecSilverRectangularPasture/USACO2020DecSilverRectangularPasture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\competitive-programming\myCpps_2020\USACO2020DecSilverRectangularPasture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D4A5414-3AB8-401C-9C97-4816786A02A1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB6EAFB3-FA30-4406-ACDF-FD2D510FD8BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12610" yWindow="0" windowWidth="3770" windowHeight="7830" firstSheet="1" activeTab="2" xr2:uid="{0B4B5404-994F-4AB5-BBE6-747CC6A3C998}"/>
+    <workbookView xWindow="14010" yWindow="0" windowWidth="3770" windowHeight="7830" firstSheet="1" activeTab="2" xr2:uid="{0B4B5404-994F-4AB5-BBE6-747CC6A3C998}"/>
   </bookViews>
   <sheets>
     <sheet name="SilverPro2.Rectangular Pasture" sheetId="1" r:id="rId1"/>
@@ -16094,17 +16094,14 @@
   <dimension ref="A1:X29"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="S8" sqref="S8"/>
+      <selection activeCell="W3" sqref="W3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.4609375" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="2.3828125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="2.4609375" style="1"/>
-    <col min="2" max="2" width="2.765625" style="16" customWidth="1"/>
-    <col min="3" max="15" width="2.765625" style="1" customWidth="1"/>
-    <col min="16" max="18" width="2.4609375" style="1"/>
-    <col min="19" max="19" width="2.84375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="16384" width="2.4609375" style="1"/>
+    <col min="1" max="1" width="2.3828125" style="1"/>
+    <col min="2" max="2" width="2.3828125" style="16"/>
+    <col min="3" max="16384" width="2.3828125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>